<commit_message>
fix problems with PPM libarary
it was a controller problem, but the PPM reader needs to know how to see it.
</commit_message>
<xml_diff>
--- a/ClubRedTape/MachineBOM.xlsx
+++ b/ClubRedTape/MachineBOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EdwardStuckey\Documents\GitHub\FightingRobot\ClubRedTape\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C953743D-F7FC-4574-A34E-65E610F33DE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0239A1E-067D-424E-9016-ACBDAD6F7CBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -106,7 +106,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="150">
   <si>
     <t>DO NOT ENTER VALUES FOR COLUMNS HIGHLIGHTED GREEN</t>
   </si>
@@ -535,6 +535,27 @@
   </si>
   <si>
     <t>#4</t>
+  </si>
+  <si>
+    <t>Alt. Club provided Drive Base motors</t>
+  </si>
+  <si>
+    <t>itgresa</t>
+  </si>
+  <si>
+    <t>Mobility (backup)</t>
+  </si>
+  <si>
+    <t>https://itgresa.com/product/turnabot-n20-motors-1400rpm/</t>
+  </si>
+  <si>
+    <t>12 Volt, 800 RPM</t>
+  </si>
+  <si>
+    <t>N20 gearmotor (alt. source)</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Thread-Rolling-Plastic-Finish-Degree/dp/B00GDYNQBM/ref=sr_1_4?crid=WPWBJQB1EK5M&amp;keywords=flat+head+thread+rolling+screw+for+plastic+%234&amp;qid=1707193390&amp;sprefix=flat+head+thread+rolling+screw+for+plastic+4%2Caps%2C87&amp;sr=8-4</t>
   </si>
 </sst>
 </file>
@@ -1017,10 +1038,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Q1010"/>
+  <dimension ref="A1:Q1011"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1067,28 +1088,28 @@
       <c r="B2" s="43"/>
       <c r="C2" s="4">
         <f>SUM(N:N)</f>
-        <v>56.454499999999996</v>
+        <v>84.354499999999987</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>2</v>
       </c>
       <c r="E2" s="4">
         <f>SUMIFS(O:O, J:J, "no")</f>
-        <v>205.96</v>
+        <v>202.96</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>3</v>
       </c>
       <c r="G2" s="4">
         <f>SUMIFS(O:O, J:J, "yes")</f>
-        <v>20.939999999999998</v>
+        <v>30.74</v>
       </c>
       <c r="H2" s="5" t="s">
         <v>4</v>
       </c>
       <c r="I2" s="4">
         <f>SUM(O:O)</f>
-        <v>226.9</v>
+        <v>233.7</v>
       </c>
       <c r="J2" s="6"/>
       <c r="K2" s="6"/>
@@ -1184,15 +1205,15 @@
         <v>87</v>
       </c>
       <c r="M4" s="2">
-        <f t="shared" ref="M4:M44" si="0">IFERROR(K4/H4, 0)</f>
+        <f t="shared" ref="M4:M45" si="0">IFERROR(K4/H4, 0)</f>
         <v>7.99</v>
       </c>
       <c r="N4" s="2">
-        <f t="shared" ref="N4:N44" si="1">I4*M4</f>
+        <f t="shared" ref="N4:N45" si="1">I4*M4</f>
         <v>7.99</v>
       </c>
       <c r="O4" s="2">
-        <f t="shared" ref="O4:O44" si="2">K4*B4</f>
+        <f t="shared" ref="O4:O45" si="2">K4*B4</f>
         <v>7.99</v>
       </c>
     </row>
@@ -1298,144 +1319,144 @@
         <v>1</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>79</v>
+        <v>148</v>
       </c>
       <c r="D7" t="s">
-        <v>80</v>
+        <v>147</v>
       </c>
       <c r="E7" t="s">
-        <v>81</v>
+        <v>143</v>
       </c>
       <c r="F7" t="s">
-        <v>77</v>
+        <v>144</v>
       </c>
       <c r="G7" s="41" t="s">
-        <v>136</v>
+        <v>146</v>
       </c>
       <c r="H7">
         <v>1</v>
       </c>
       <c r="I7">
+        <v>3</v>
+      </c>
+      <c r="J7" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="K7" s="12">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="L7" s="31" t="s">
+        <v>145</v>
+      </c>
+      <c r="M7" s="2">
+        <f t="shared" ref="M7" si="3">IFERROR(K7/H7, 0)</f>
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="N7" s="2">
+        <f t="shared" ref="N7" si="4">I7*M7</f>
+        <v>29.400000000000002</v>
+      </c>
+      <c r="O7" s="2">
+        <f t="shared" ref="O7" si="5">K7*B7</f>
+        <v>9.8000000000000007</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A8" s="8"/>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="D8" t="s">
+        <v>80</v>
+      </c>
+      <c r="E8" t="s">
+        <v>81</v>
+      </c>
+      <c r="F8" t="s">
+        <v>77</v>
+      </c>
+      <c r="G8" s="41" t="s">
+        <v>136</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
         <v>2</v>
       </c>
-      <c r="J7" s="34" t="s">
+      <c r="J8" s="34" t="s">
         <v>78</v>
       </c>
-      <c r="K7" s="12">
+      <c r="K8" s="12">
         <v>1.66</v>
       </c>
-      <c r="L7" s="31" t="s">
+      <c r="L8" s="31" t="s">
         <v>90</v>
       </c>
-      <c r="M7" s="2">
+      <c r="M8" s="2">
         <f t="shared" si="0"/>
         <v>1.66</v>
       </c>
-      <c r="N7" s="2">
+      <c r="N8" s="2">
         <f t="shared" si="1"/>
         <v>3.32</v>
       </c>
-      <c r="O7" s="2">
+      <c r="O8" s="2">
         <f t="shared" si="2"/>
         <v>1.66</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A8" s="8" t="s">
+    <row r="9" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A9" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B8">
+      <c r="B9">
         <v>1</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C9" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D9" t="s">
         <v>83</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E9" t="s">
         <v>84</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F9" t="s">
         <v>27</v>
       </c>
-      <c r="G8" s="41" t="s">
+      <c r="G9" s="41" t="s">
         <v>137</v>
       </c>
-      <c r="H8">
+      <c r="H9">
         <v>4</v>
       </c>
-      <c r="I8">
+      <c r="I9">
         <v>1</v>
       </c>
-      <c r="J8" s="34" t="s">
+      <c r="J9" s="34" t="s">
         <v>78</v>
       </c>
-      <c r="K8" s="12">
+      <c r="K9" s="12">
         <v>30</v>
       </c>
-      <c r="L8" s="31" t="s">
+      <c r="L9" s="31" t="s">
         <v>91</v>
       </c>
-      <c r="M8" s="2">
+      <c r="M9" s="2">
         <f t="shared" si="0"/>
         <v>7.5</v>
       </c>
-      <c r="N8" s="2">
+      <c r="N9" s="2">
         <f t="shared" si="1"/>
         <v>7.5</v>
       </c>
-      <c r="O8" s="2">
+      <c r="O9" s="2">
         <f t="shared" si="2"/>
         <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A9" s="8"/>
-      <c r="B9">
-        <v>1</v>
-      </c>
-      <c r="C9" s="32" t="s">
-        <v>92</v>
-      </c>
-      <c r="D9" s="31" t="s">
-        <v>93</v>
-      </c>
-      <c r="E9" s="31" t="s">
-        <v>94</v>
-      </c>
-      <c r="F9" s="31" t="s">
-        <v>27</v>
-      </c>
-      <c r="G9" s="41" t="s">
-        <v>141</v>
-      </c>
-      <c r="H9">
-        <v>4</v>
-      </c>
-      <c r="I9">
-        <v>1</v>
-      </c>
-      <c r="J9" s="34" t="s">
-        <v>78</v>
-      </c>
-      <c r="K9" s="12">
-        <v>31.99</v>
-      </c>
-      <c r="L9" s="31" t="s">
-        <v>51</v>
-      </c>
-      <c r="M9" s="2">
-        <f t="shared" si="0"/>
-        <v>7.9974999999999996</v>
-      </c>
-      <c r="N9" s="2">
-        <f t="shared" si="1"/>
-        <v>7.9974999999999996</v>
-      </c>
-      <c r="O9" s="2">
-        <f t="shared" si="2"/>
-        <v>31.99</v>
       </c>
     </row>
     <row r="10" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
@@ -1443,44 +1464,47 @@
       <c r="B10">
         <v>1</v>
       </c>
-      <c r="C10" s="10" t="s">
-        <v>31</v>
+      <c r="C10" s="32" t="s">
+        <v>92</v>
       </c>
       <c r="D10" s="31" t="s">
-        <v>98</v>
-      </c>
-      <c r="E10" t="s">
-        <v>85</v>
+        <v>93</v>
+      </c>
+      <c r="E10" s="31" t="s">
+        <v>94</v>
       </c>
       <c r="F10" s="31" t="s">
-        <v>96</v>
+        <v>27</v>
+      </c>
+      <c r="G10" s="41" t="s">
+        <v>141</v>
       </c>
       <c r="H10">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I10">
-        <v>2</v>
-      </c>
-      <c r="J10" s="28" t="s">
-        <v>24</v>
+        <v>1</v>
+      </c>
+      <c r="J10" s="34" t="s">
+        <v>78</v>
       </c>
       <c r="K10" s="12">
-        <v>0</v>
+        <v>31.99</v>
       </c>
       <c r="L10" s="31" t="s">
-        <v>87</v>
+        <v>51</v>
       </c>
       <c r="M10" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>7.9974999999999996</v>
       </c>
       <c r="N10" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>7.9974999999999996</v>
       </c>
       <c r="O10" s="2">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>31.99</v>
       </c>
     </row>
     <row r="11" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
@@ -1488,47 +1512,44 @@
       <c r="B11">
         <v>1</v>
       </c>
-      <c r="C11" s="32" t="s">
-        <v>99</v>
+      <c r="C11" s="10" t="s">
+        <v>31</v>
       </c>
       <c r="D11" s="31" t="s">
-        <v>100</v>
-      </c>
-      <c r="E11" s="31" t="s">
-        <v>76</v>
+        <v>98</v>
+      </c>
+      <c r="E11" t="s">
+        <v>85</v>
       </c>
       <c r="F11" s="31" t="s">
-        <v>77</v>
-      </c>
-      <c r="G11" s="41" t="s">
-        <v>139</v>
+        <v>96</v>
       </c>
       <c r="H11">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="I11">
         <v>2</v>
       </c>
-      <c r="J11" s="34" t="s">
-        <v>78</v>
+      <c r="J11" s="28" t="s">
+        <v>24</v>
       </c>
       <c r="K11" s="12">
-        <v>4.6399999999999997</v>
+        <v>0</v>
       </c>
       <c r="L11" s="31" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="M11" s="2">
-        <f t="shared" ref="M11:M12" si="3">IFERROR(K11/H11, 0)</f>
-        <v>0.46399999999999997</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="N11" s="2">
-        <f t="shared" ref="N11:N12" si="4">I11*M11</f>
-        <v>0.92799999999999994</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="O11" s="2">
-        <f t="shared" ref="O11:O12" si="5">K11*B11</f>
-        <v>4.6399999999999997</v>
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
@@ -1537,46 +1558,46 @@
         <v>1</v>
       </c>
       <c r="C12" s="32" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D12" s="31" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E12" s="31" t="s">
-        <v>106</v>
+        <v>76</v>
       </c>
       <c r="F12" s="31" t="s">
-        <v>27</v>
+        <v>77</v>
       </c>
       <c r="G12" s="41" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="H12">
         <v>10</v>
       </c>
       <c r="I12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J12" s="34" t="s">
         <v>78</v>
       </c>
       <c r="K12" s="12">
-        <v>14</v>
+        <v>4.6399999999999997</v>
       </c>
       <c r="L12" s="31" t="s">
-        <v>118</v>
+        <v>89</v>
       </c>
       <c r="M12" s="2">
-        <f t="shared" si="3"/>
-        <v>1.4</v>
+        <f t="shared" ref="M12:M13" si="6">IFERROR(K12/H12, 0)</f>
+        <v>0.46399999999999997</v>
       </c>
       <c r="N12" s="2">
-        <f t="shared" si="4"/>
-        <v>1.4</v>
+        <f t="shared" ref="N12:N13" si="7">I12*M12</f>
+        <v>0.92799999999999994</v>
       </c>
       <c r="O12" s="2">
-        <f t="shared" si="5"/>
-        <v>14</v>
+        <f t="shared" ref="O12:O13" si="8">K12*B12</f>
+        <v>4.6399999999999997</v>
       </c>
     </row>
     <row r="13" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
@@ -1585,22 +1606,22 @@
         <v>1</v>
       </c>
       <c r="C13" s="32" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D13" s="31" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E13" s="31" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="F13" s="31" t="s">
-        <v>77</v>
+        <v>27</v>
       </c>
       <c r="G13" s="41" t="s">
-        <v>129</v>
+        <v>138</v>
       </c>
       <c r="H13">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="I13">
         <v>1</v>
@@ -1609,22 +1630,22 @@
         <v>78</v>
       </c>
       <c r="K13" s="12">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="L13" s="31" t="s">
         <v>118</v>
       </c>
       <c r="M13" s="2">
-        <f t="shared" si="0"/>
-        <v>0.1</v>
+        <f t="shared" si="6"/>
+        <v>1.4</v>
       </c>
       <c r="N13" s="2">
-        <f t="shared" si="1"/>
-        <v>0.1</v>
+        <f t="shared" si="7"/>
+        <v>1.4</v>
       </c>
       <c r="O13" s="2">
-        <f t="shared" si="2"/>
-        <v>2</v>
+        <f t="shared" si="8"/>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
@@ -1633,22 +1654,22 @@
         <v>1</v>
       </c>
       <c r="C14" s="32" t="s">
-        <v>119</v>
+        <v>102</v>
       </c>
       <c r="D14" s="31" t="s">
-        <v>121</v>
+        <v>104</v>
       </c>
       <c r="E14" s="31" t="s">
-        <v>122</v>
+        <v>105</v>
       </c>
       <c r="F14" s="31" t="s">
         <v>77</v>
       </c>
       <c r="G14" s="41" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="H14">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="I14">
         <v>1</v>
@@ -1657,22 +1678,22 @@
         <v>78</v>
       </c>
       <c r="K14" s="12">
-        <v>2.12</v>
+        <v>2</v>
       </c>
       <c r="L14" s="31" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="M14" s="2">
-        <f t="shared" ref="M14:M16" si="6">IFERROR(K14/H14, 0)</f>
-        <v>2.12</v>
+        <f t="shared" si="0"/>
+        <v>0.1</v>
       </c>
       <c r="N14" s="2">
-        <f t="shared" ref="N14:N16" si="7">I14*M14</f>
-        <v>2.12</v>
+        <f t="shared" si="1"/>
+        <v>0.1</v>
       </c>
       <c r="O14" s="2">
-        <f t="shared" ref="O14:O16" si="8">K14*B14</f>
-        <v>2.12</v>
+        <f t="shared" si="2"/>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
@@ -1681,22 +1702,22 @@
         <v>1</v>
       </c>
       <c r="C15" s="32" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>121</v>
       </c>
       <c r="E15" s="31" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F15" s="31" t="s">
         <v>77</v>
       </c>
       <c r="G15" s="41" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="H15">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="I15">
         <v>1</v>
@@ -1705,22 +1726,22 @@
         <v>78</v>
       </c>
       <c r="K15" s="12">
-        <v>14</v>
-      </c>
-      <c r="L15" t="s">
-        <v>90</v>
+        <v>2.12</v>
+      </c>
+      <c r="L15" s="31" t="s">
+        <v>127</v>
       </c>
       <c r="M15" s="2">
-        <f t="shared" si="6"/>
-        <v>1.4</v>
+        <f t="shared" ref="M15:M17" si="9">IFERROR(K15/H15, 0)</f>
+        <v>2.12</v>
       </c>
       <c r="N15" s="2">
-        <f t="shared" si="7"/>
-        <v>1.4</v>
+        <f t="shared" ref="N15:N17" si="10">I15*M15</f>
+        <v>2.12</v>
       </c>
       <c r="O15" s="2">
-        <f t="shared" si="8"/>
-        <v>14</v>
+        <f t="shared" ref="O15:O17" si="11">K15*B15</f>
+        <v>2.12</v>
       </c>
     </row>
     <row r="16" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
@@ -1728,156 +1749,175 @@
       <c r="B16">
         <v>1</v>
       </c>
-      <c r="C16" s="39" t="s">
-        <v>130</v>
-      </c>
-      <c r="D16" s="36" t="s">
-        <v>131</v>
-      </c>
-      <c r="E16" s="36" t="s">
-        <v>132</v>
-      </c>
-      <c r="F16" s="36" t="s">
+      <c r="C16" s="32" t="s">
+        <v>120</v>
+      </c>
+      <c r="D16" s="31" t="s">
+        <v>121</v>
+      </c>
+      <c r="E16" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="F16" s="31" t="s">
         <v>77</v>
       </c>
       <c r="G16" s="41" t="s">
-        <v>133</v>
-      </c>
-      <c r="H16" s="36">
+        <v>134</v>
+      </c>
+      <c r="H16">
         <v>10</v>
       </c>
-      <c r="I16" s="36">
-        <v>2</v>
+      <c r="I16">
+        <v>1</v>
       </c>
       <c r="J16" s="34" t="s">
         <v>78</v>
       </c>
       <c r="K16" s="12">
+        <v>14</v>
+      </c>
+      <c r="L16" t="s">
+        <v>90</v>
+      </c>
+      <c r="M16" s="2">
+        <f t="shared" si="9"/>
+        <v>1.4</v>
+      </c>
+      <c r="N16" s="2">
+        <f t="shared" si="10"/>
+        <v>1.4</v>
+      </c>
+      <c r="O16" s="2">
+        <f t="shared" si="11"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A17" s="8"/>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17" s="39" t="s">
+        <v>130</v>
+      </c>
+      <c r="D17" s="36" t="s">
+        <v>131</v>
+      </c>
+      <c r="E17" s="36" t="s">
+        <v>132</v>
+      </c>
+      <c r="F17" s="36" t="s">
+        <v>77</v>
+      </c>
+      <c r="G17" s="41" t="s">
+        <v>133</v>
+      </c>
+      <c r="H17" s="36">
+        <v>10</v>
+      </c>
+      <c r="I17" s="36">
+        <v>2</v>
+      </c>
+      <c r="J17" s="34" t="s">
+        <v>78</v>
+      </c>
+      <c r="K17" s="12">
         <v>16.37</v>
       </c>
-      <c r="L16" t="s">
+      <c r="L17" t="s">
         <v>51</v>
       </c>
-      <c r="M16" s="2">
-        <f t="shared" si="6"/>
+      <c r="M17" s="2">
+        <f t="shared" si="9"/>
         <v>1.637</v>
       </c>
-      <c r="N16" s="2">
-        <f t="shared" si="7"/>
+      <c r="N17" s="2">
+        <f t="shared" si="10"/>
         <v>3.274</v>
       </c>
-      <c r="O16" s="2">
-        <f t="shared" si="8"/>
+      <c r="O17" s="2">
+        <f t="shared" si="11"/>
         <v>16.37</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A17" s="13"/>
-      <c r="C17" s="36" t="s">
+    <row r="18" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A18" s="13"/>
+      <c r="C18" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="D17" s="36"/>
-      <c r="E17" s="36"/>
-      <c r="F17" s="36"/>
-      <c r="G17" s="36"/>
-      <c r="H17" s="36"/>
-      <c r="I17" s="36"/>
-      <c r="J17" s="36"/>
-      <c r="K17" s="12">
-        <v>0</v>
-      </c>
-      <c r="M17" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="N17" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O17" s="2">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A18" s="13"/>
-      <c r="B18">
-        <v>1</v>
-      </c>
-      <c r="C18" s="36" t="s">
-        <v>73</v>
-      </c>
-      <c r="D18" s="36" t="s">
-        <v>126</v>
-      </c>
-      <c r="E18" s="36" t="s">
-        <v>125</v>
-      </c>
-      <c r="F18" s="36" t="s">
-        <v>124</v>
-      </c>
+      <c r="D18" s="36"/>
+      <c r="E18" s="36"/>
+      <c r="F18" s="36"/>
       <c r="G18" s="36"/>
-      <c r="H18" s="36">
-        <v>50</v>
-      </c>
-      <c r="I18" s="36">
-        <v>0.5</v>
-      </c>
-      <c r="J18" s="34" t="s">
-        <v>78</v>
-      </c>
+      <c r="H18" s="36"/>
+      <c r="I18" s="36"/>
+      <c r="J18" s="36"/>
       <c r="K18" s="12">
-        <v>80</v>
-      </c>
-      <c r="L18" s="31" t="s">
-        <v>117</v>
+        <v>0</v>
       </c>
       <c r="M18" s="2">
         <f t="shared" si="0"/>
-        <v>1.6</v>
+        <v>0</v>
       </c>
       <c r="N18" s="2">
         <f t="shared" si="1"/>
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="O18" s="2">
         <f t="shared" si="2"/>
-        <v>80</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A19" s="13" t="s">
-        <v>33</v>
-      </c>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A19" s="13"/>
       <c r="B19">
         <v>1</v>
       </c>
-      <c r="C19" s="36"/>
-      <c r="D19" s="36"/>
-      <c r="E19" s="36"/>
-      <c r="F19" s="36"/>
+      <c r="C19" s="36" t="s">
+        <v>73</v>
+      </c>
+      <c r="D19" s="36" t="s">
+        <v>126</v>
+      </c>
+      <c r="E19" s="36" t="s">
+        <v>125</v>
+      </c>
+      <c r="F19" s="36" t="s">
+        <v>124</v>
+      </c>
       <c r="G19" s="36"/>
-      <c r="H19" s="36"/>
-      <c r="I19" s="36"/>
-      <c r="J19" s="36"/>
+      <c r="H19" s="36">
+        <v>50</v>
+      </c>
+      <c r="I19" s="36">
+        <v>0.5</v>
+      </c>
+      <c r="J19" s="34" t="s">
+        <v>78</v>
+      </c>
       <c r="K19" s="12">
-        <v>0</v>
+        <v>80</v>
+      </c>
+      <c r="L19" s="31" t="s">
+        <v>117</v>
       </c>
       <c r="M19" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.6</v>
       </c>
       <c r="N19" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="O19" s="2">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>80</v>
       </c>
     </row>
     <row r="20" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A20" s="13"/>
+      <c r="A20" s="13" t="s">
+        <v>33</v>
+      </c>
       <c r="B20">
         <v>1</v>
       </c>
@@ -1935,22 +1975,21 @@
       </c>
     </row>
     <row r="22" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A22" s="14"/>
-      <c r="B22" s="30"/>
-      <c r="C22" s="37" t="s">
-        <v>34</v>
-      </c>
-      <c r="D22" s="37"/>
-      <c r="E22" s="37"/>
-      <c r="F22" s="37"/>
-      <c r="G22" s="37"/>
-      <c r="H22" s="38"/>
-      <c r="I22" s="38"/>
+      <c r="A22" s="13"/>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22" s="36"/>
+      <c r="D22" s="36"/>
+      <c r="E22" s="36"/>
+      <c r="F22" s="36"/>
+      <c r="G22" s="36"/>
+      <c r="H22" s="36"/>
+      <c r="I22" s="36"/>
       <c r="J22" s="36"/>
       <c r="K22" s="12">
         <v>0</v>
       </c>
-      <c r="L22" s="29"/>
       <c r="M22" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1964,80 +2003,60 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="14"/>
-      <c r="B23">
-        <v>1</v>
-      </c>
-      <c r="C23" s="36" t="s">
-        <v>95</v>
-      </c>
-      <c r="D23" s="36" t="s">
-        <v>109</v>
-      </c>
-      <c r="E23" s="36" t="s">
-        <v>111</v>
-      </c>
-      <c r="F23" s="36" t="s">
-        <v>113</v>
-      </c>
-      <c r="G23" s="36" t="s">
-        <v>114</v>
-      </c>
-      <c r="H23" s="36">
-        <v>100</v>
-      </c>
-      <c r="I23" s="36">
-        <v>3</v>
-      </c>
-      <c r="J23" s="34" t="s">
-        <v>78</v>
-      </c>
+      <c r="B23" s="30"/>
+      <c r="C23" s="37" t="s">
+        <v>34</v>
+      </c>
+      <c r="D23" s="37"/>
+      <c r="E23" s="37"/>
+      <c r="F23" s="37"/>
+      <c r="G23" s="37"/>
+      <c r="H23" s="38"/>
+      <c r="I23" s="38"/>
+      <c r="J23" s="36"/>
       <c r="K23" s="12">
-        <v>2.25</v>
-      </c>
-      <c r="L23" s="31" t="s">
-        <v>116</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="L23" s="29"/>
       <c r="M23" s="2">
         <f t="shared" si="0"/>
-        <v>2.2499999999999999E-2</v>
+        <v>0</v>
       </c>
       <c r="N23" s="2">
         <f t="shared" si="1"/>
-        <v>6.7500000000000004E-2</v>
+        <v>0</v>
       </c>
       <c r="O23" s="2">
         <f t="shared" si="2"/>
-        <v>2.25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A24" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="B24" s="30">
+      <c r="A24" s="14"/>
+      <c r="B24">
         <v>1</v>
       </c>
-      <c r="C24" s="37" t="s">
-        <v>107</v>
-      </c>
-      <c r="D24" s="37" t="s">
-        <v>110</v>
-      </c>
-      <c r="E24" s="37" t="s">
-        <v>112</v>
-      </c>
-      <c r="F24" s="37" t="s">
+      <c r="C24" s="36" t="s">
+        <v>95</v>
+      </c>
+      <c r="D24" s="36" t="s">
+        <v>109</v>
+      </c>
+      <c r="E24" s="36" t="s">
+        <v>111</v>
+      </c>
+      <c r="F24" s="36" t="s">
         <v>113</v>
       </c>
-      <c r="G24" s="37" t="s">
-        <v>115</v>
-      </c>
-      <c r="H24" s="38">
+      <c r="G24" s="36" t="s">
+        <v>114</v>
+      </c>
+      <c r="H24" s="36">
         <v>100</v>
       </c>
-      <c r="I24" s="38">
+      <c r="I24" s="36">
         <v>3</v>
       </c>
       <c r="J24" s="34" t="s">
@@ -2046,7 +2065,7 @@
       <c r="K24" s="12">
         <v>2.25</v>
       </c>
-      <c r="L24" s="40" t="s">
+      <c r="L24" s="31" t="s">
         <v>116</v>
       </c>
       <c r="M24" s="2">
@@ -2063,65 +2082,89 @@
       </c>
     </row>
     <row r="25" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A25" s="14"/>
-      <c r="B25">
+      <c r="A25" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B25" s="30">
         <v>1</v>
       </c>
-      <c r="C25" s="36" t="s">
-        <v>108</v>
-      </c>
-      <c r="D25" s="36" t="s">
-        <v>142</v>
-      </c>
-      <c r="E25" s="36" t="s">
-        <v>128</v>
-      </c>
-      <c r="F25" s="36" t="s">
+      <c r="C25" s="37" t="s">
+        <v>107</v>
+      </c>
+      <c r="D25" s="37" t="s">
+        <v>110</v>
+      </c>
+      <c r="E25" s="37" t="s">
+        <v>112</v>
+      </c>
+      <c r="F25" s="37" t="s">
         <v>113</v>
       </c>
-      <c r="G25" s="36" t="s">
+      <c r="G25" s="37" t="s">
         <v>115</v>
       </c>
-      <c r="H25" s="36">
+      <c r="H25" s="38">
         <v>100</v>
       </c>
-      <c r="I25" s="36">
-        <v>50</v>
+      <c r="I25" s="38">
+        <v>3</v>
       </c>
       <c r="J25" s="34" t="s">
         <v>78</v>
       </c>
       <c r="K25" s="12">
-        <v>3</v>
+        <v>2.25</v>
       </c>
       <c r="L25" s="40" t="s">
         <v>116</v>
       </c>
       <c r="M25" s="2">
         <f t="shared" si="0"/>
-        <v>0.03</v>
+        <v>2.2499999999999999E-2</v>
       </c>
       <c r="N25" s="2">
         <f t="shared" si="1"/>
-        <v>1.5</v>
+        <v>6.7500000000000004E-2</v>
       </c>
       <c r="O25" s="2">
         <f t="shared" si="2"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
+        <v>2.25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A26" s="14"/>
-      <c r="C26" s="36"/>
-      <c r="D26" s="36"/>
-      <c r="E26" s="36"/>
-      <c r="F26" s="36"/>
-      <c r="G26" s="36"/>
-      <c r="H26" s="36"/>
-      <c r="I26" s="36"/>
-      <c r="J26" s="36"/>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26" s="36" t="s">
+        <v>108</v>
+      </c>
+      <c r="D26" s="36" t="s">
+        <v>142</v>
+      </c>
+      <c r="E26" s="36" t="s">
+        <v>128</v>
+      </c>
+      <c r="F26" s="36" t="s">
+        <v>27</v>
+      </c>
+      <c r="G26" s="41" t="s">
+        <v>149</v>
+      </c>
+      <c r="H26" s="36">
+        <v>100</v>
+      </c>
+      <c r="I26" s="36">
+        <v>50</v>
+      </c>
+      <c r="J26" s="28" t="s">
+        <v>24</v>
+      </c>
       <c r="K26" s="12">
         <v>0</v>
+      </c>
+      <c r="L26" s="40" t="s">
+        <v>116</v>
       </c>
       <c r="M26" s="2">
         <f t="shared" si="0"/>
@@ -2137,10 +2180,8 @@
       </c>
     </row>
     <row r="27" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A27" s="15"/>
-      <c r="C27" s="36" t="s">
-        <v>36</v>
-      </c>
+      <c r="A27" s="14"/>
+      <c r="C27" s="36"/>
       <c r="D27" s="36"/>
       <c r="E27" s="36"/>
       <c r="F27" s="36"/>
@@ -2166,7 +2207,9 @@
     </row>
     <row r="28" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="15"/>
-      <c r="C28" s="36"/>
+      <c r="C28" s="36" t="s">
+        <v>36</v>
+      </c>
       <c r="D28" s="36"/>
       <c r="E28" s="36"/>
       <c r="F28" s="36"/>
@@ -2191,9 +2234,7 @@
       </c>
     </row>
     <row r="29" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A29" s="15" t="s">
-        <v>37</v>
-      </c>
+      <c r="A29" s="15"/>
       <c r="C29" s="36"/>
       <c r="D29" s="36"/>
       <c r="E29" s="36"/>
@@ -2219,7 +2260,9 @@
       </c>
     </row>
     <row r="30" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A30" s="15"/>
+      <c r="A30" s="15" t="s">
+        <v>37</v>
+      </c>
       <c r="C30" s="36"/>
       <c r="D30" s="36"/>
       <c r="E30" s="36"/>
@@ -2271,6 +2314,7 @@
       </c>
     </row>
     <row r="32" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A32" s="15"/>
       <c r="C32" s="36"/>
       <c r="D32" s="36"/>
       <c r="E32" s="36"/>
@@ -2571,6 +2615,14 @@
       </c>
     </row>
     <row r="44" spans="3:15" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C44" s="36"/>
+      <c r="D44" s="36"/>
+      <c r="E44" s="36"/>
+      <c r="F44" s="36"/>
+      <c r="G44" s="36"/>
+      <c r="H44" s="36"/>
+      <c r="I44" s="36"/>
+      <c r="J44" s="36"/>
       <c r="K44" s="12">
         <v>0</v>
       </c>
@@ -2588,9 +2640,21 @@
       </c>
     </row>
     <row r="45" spans="3:15" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="M45" s="2"/>
-      <c r="N45" s="1"/>
-      <c r="O45" s="1"/>
+      <c r="K45" s="12">
+        <v>0</v>
+      </c>
+      <c r="M45" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N45" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O45" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="46" spans="3:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="M46" s="2"/>
@@ -7416,32 +7480,39 @@
       <c r="M1010" s="2"/>
       <c r="N1010" s="1"/>
       <c r="O1010" s="1"/>
+    </row>
+    <row r="1011" spans="13:15" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="M1011" s="2"/>
+      <c r="N1011" s="1"/>
+      <c r="O1011" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A2:B2"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="J17:J31 J4:J15" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="J18:J32 J4:J16" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"yes,no"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="G4" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="G5" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="G13" r:id="rId3" xr:uid="{D3C6BCA6-BD7A-48E4-87B0-DC852AE79F27}"/>
-    <hyperlink ref="G16" r:id="rId4" xr:uid="{957F53B9-7A9D-4AF3-8684-7507A722D2CD}"/>
-    <hyperlink ref="G15" r:id="rId5" display="https://www.aliexpress.us/item/3256806245533637.html?spm=a2g0o.productlist.main.7.f4bc1f0fLfa4gv&amp;algo_pvid=46fa75e4-e21d-4e65-8d48-c4104720264a&amp;algo_exp_id=46fa75e4-e21d-4e65-8d48-c4104720264a-3&amp;pdp_npi=4%40dis%21USD%214.67%210.99%21%21%2133.50%217.05%21%402103243417078697094002440e13f8%2112000037156177261%21sea%21US%210%21AB&amp;curPageLogUid=V13r8UBbxRr8&amp;utparam-url=scene%3Asearch%7Cquery_from%3A" xr:uid="{FAEC0219-6298-4D04-B71D-06FEE197AA7E}"/>
-    <hyperlink ref="G14" r:id="rId6" xr:uid="{BA6BFFCF-0C08-490A-B900-5820C9591119}"/>
-    <hyperlink ref="G7" r:id="rId7" xr:uid="{9E6DA463-521E-4A32-952B-B828ECE1464A}"/>
-    <hyperlink ref="G8" r:id="rId8" xr:uid="{E9A398C1-724A-4DA7-90B9-506F9EF964D0}"/>
-    <hyperlink ref="G12" r:id="rId9" xr:uid="{0A67941F-87C4-4A6E-9219-BD02B31B9D96}"/>
-    <hyperlink ref="G11" r:id="rId10" xr:uid="{C935F81F-3C2D-4DDB-83F5-D3E0F4AE15E5}"/>
+    <hyperlink ref="G14" r:id="rId3" xr:uid="{D3C6BCA6-BD7A-48E4-87B0-DC852AE79F27}"/>
+    <hyperlink ref="G17" r:id="rId4" xr:uid="{957F53B9-7A9D-4AF3-8684-7507A722D2CD}"/>
+    <hyperlink ref="G16" r:id="rId5" display="https://www.aliexpress.us/item/3256806245533637.html?spm=a2g0o.productlist.main.7.f4bc1f0fLfa4gv&amp;algo_pvid=46fa75e4-e21d-4e65-8d48-c4104720264a&amp;algo_exp_id=46fa75e4-e21d-4e65-8d48-c4104720264a-3&amp;pdp_npi=4%40dis%21USD%214.67%210.99%21%21%2133.50%217.05%21%402103243417078697094002440e13f8%2112000037156177261%21sea%21US%210%21AB&amp;curPageLogUid=V13r8UBbxRr8&amp;utparam-url=scene%3Asearch%7Cquery_from%3A" xr:uid="{FAEC0219-6298-4D04-B71D-06FEE197AA7E}"/>
+    <hyperlink ref="G15" r:id="rId6" xr:uid="{BA6BFFCF-0C08-490A-B900-5820C9591119}"/>
+    <hyperlink ref="G8" r:id="rId7" xr:uid="{9E6DA463-521E-4A32-952B-B828ECE1464A}"/>
+    <hyperlink ref="G9" r:id="rId8" xr:uid="{E9A398C1-724A-4DA7-90B9-506F9EF964D0}"/>
+    <hyperlink ref="G13" r:id="rId9" xr:uid="{0A67941F-87C4-4A6E-9219-BD02B31B9D96}"/>
+    <hyperlink ref="G12" r:id="rId10" xr:uid="{C935F81F-3C2D-4DDB-83F5-D3E0F4AE15E5}"/>
     <hyperlink ref="G6" r:id="rId11" xr:uid="{B3E5A1E9-CC14-4749-9A21-DF45016DEF82}"/>
-    <hyperlink ref="G9" r:id="rId12" xr:uid="{75D8582E-F0E9-4F68-BC5C-55DD2825AA2E}"/>
+    <hyperlink ref="G10" r:id="rId12" xr:uid="{75D8582E-F0E9-4F68-BC5C-55DD2825AA2E}"/>
+    <hyperlink ref="G7" r:id="rId13" xr:uid="{A4366310-A20D-44FF-A4C5-AE1EB0A9F48E}"/>
+    <hyperlink ref="G26" r:id="rId14" xr:uid="{0865EF66-CB85-46F1-BC7C-A8208D7E6BFE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId13"/>
+  <legacyDrawing r:id="rId15"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
initial outlier processing removal
still exist in-code, but is commented out
</commit_message>
<xml_diff>
--- a/ClubRedTape/MachineBOM.xlsx
+++ b/ClubRedTape/MachineBOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EdwardStuckey\Documents\GitHub\FightingRobot\ClubRedTape\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0239A1E-067D-424E-9016-ACBDAD6F7CBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D29C87B5-3B75-47B8-BBAE-DFDF29CF6B6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1041,7 +1041,7 @@
   <dimension ref="A1:Q1011"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>